<commit_message>
Creating Health system + Splitting scripts I
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdunn9\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charm\Workspace\Game Dev I (AGA206)\Roll-A-Ball-Sep-24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B03DEA0-075E-4830-9338-695C6405FD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C409F7FF-1237-49B6-851F-C4B14BE6713D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="2520" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>AGA206 Assessment 2 Checklist</t>
   </si>
@@ -142,6 +153,28 @@
   </si>
   <si>
     <t>Joshua Dunn</t>
+  </si>
+  <si>
+    <t>This Week</t>
+  </si>
+  <si>
+    <t>Sketches / Plans for Levels</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This Week </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tonight</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -308,7 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -388,23 +421,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -525,7 +541,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$38" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$39" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -533,7 +549,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$15" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$15" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2499,10 +2515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:L39"/>
+  <dimension ref="B2:L40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:G5"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2567,15 +2583,16 @@
       </c>
       <c r="D7" s="8">
         <f>COUNTIFS(J12:J15,TRUE)</f>
-        <v>3</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="G7"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="8">
-        <f>COUNTIFS(J18:J38,TRUE)</f>
+        <f>COUNTIFS(J18:J39,TRUE)</f>
         <v>0</v>
       </c>
     </row>
@@ -2584,7 +2601,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="8">
-        <f>K39</f>
+        <f>K40</f>
         <v>0</v>
       </c>
     </row>
@@ -2682,11 +2699,11 @@
       <c r="E15" s="7"/>
       <c r="F15" s="6" t="str">
         <f>IF(J15,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G15" s="17"/>
       <c r="J15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2711,21 +2728,23 @@
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="29">
+      <c r="B18" s="6">
         <v>5</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="31">
+      <c r="D18" s="19">
         <v>2</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="29" t="str">
+      <c r="E18" s="7"/>
+      <c r="F18" s="6" t="str">
         <f t="shared" ref="F18:F35" si="0">IF(J18,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="G18" s="33"/>
+      <c r="G18" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="J18" s="5" t="b">
         <v>0</v>
       </c>
@@ -2749,31 +2768,33 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G19" s="17"/>
+      <c r="G19" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="J19" s="5" t="b">
         <v>0</v>
       </c>
       <c r="K19" s="2">
-        <f t="shared" ref="K19:K38" si="1">IF(J19=TRUE,D19,0)</f>
+        <f t="shared" ref="K19:K39" si="1">IF(J19=TRUE,D19,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="29">
+      <c r="B20" s="6">
         <v>7</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="31">
+      <c r="D20" s="19">
         <v>2</v>
       </c>
-      <c r="E20" s="32"/>
-      <c r="F20" s="29" t="str">
+      <c r="E20" s="7"/>
+      <c r="F20" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G20" s="33"/>
+      <c r="G20" s="17"/>
       <c r="J20" s="5" t="b">
         <v>0</v>
       </c>
@@ -2783,21 +2804,23 @@
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="29">
+      <c r="B21" s="6">
         <v>8</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="19">
         <v>2</v>
       </c>
-      <c r="E21" s="32"/>
-      <c r="F21" s="29" t="str">
+      <c r="E21" s="7"/>
+      <c r="F21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G21" s="33"/>
+      <c r="G21" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="J21" s="5" t="b">
         <v>0</v>
       </c>
@@ -2807,21 +2830,23 @@
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="29">
+      <c r="B22" s="6">
         <v>9</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D22" s="19">
         <v>1</v>
       </c>
-      <c r="E22" s="32"/>
-      <c r="F22" s="29" t="str">
+      <c r="E22" s="7"/>
+      <c r="F22" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G22" s="33"/>
+      <c r="G22" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="J22" s="5" t="b">
         <v>0</v>
       </c>
@@ -2831,21 +2856,23 @@
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="29">
+      <c r="B23" s="6">
         <v>10</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="31">
+      <c r="D23" s="19">
         <v>1</v>
       </c>
-      <c r="E23" s="32"/>
-      <c r="F23" s="29" t="str">
+      <c r="E23" s="7"/>
+      <c r="F23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G23" s="33"/>
+      <c r="G23" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="J23" s="5" t="b">
         <v>0</v>
       </c>
@@ -2855,21 +2882,23 @@
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="29">
+      <c r="B24" s="6">
         <v>11</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="19">
         <v>1</v>
       </c>
-      <c r="E24" s="32"/>
-      <c r="F24" s="29" t="str">
+      <c r="E24" s="7"/>
+      <c r="F24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G24" s="33"/>
+      <c r="G24" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="J24" s="5" t="b">
         <v>0</v>
       </c>
@@ -2879,21 +2908,23 @@
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="29">
+      <c r="B25" s="6">
         <v>12</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="31">
+      <c r="D25" s="19">
         <v>1</v>
       </c>
-      <c r="E25" s="32"/>
-      <c r="F25" s="29" t="str">
+      <c r="E25" s="7"/>
+      <c r="F25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G25" s="33"/>
+      <c r="G25" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="J25" s="5" t="b">
         <v>0</v>
       </c>
@@ -2903,21 +2934,21 @@
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="29">
+      <c r="B26" s="6">
         <v>13</v>
       </c>
-      <c r="C26" s="30" t="s">
+      <c r="C26" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="31">
+      <c r="D26" s="19">
         <v>1</v>
       </c>
-      <c r="E26" s="32"/>
-      <c r="F26" s="29" t="str">
+      <c r="E26" s="7"/>
+      <c r="F26" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G26" s="33"/>
+      <c r="G26" s="17"/>
       <c r="J26" s="5" t="b">
         <v>0</v>
       </c>
@@ -2927,21 +2958,21 @@
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="29">
+      <c r="B27" s="6">
         <v>14</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="31">
+      <c r="D27" s="19">
         <v>1</v>
       </c>
-      <c r="E27" s="32"/>
-      <c r="F27" s="29" t="str">
+      <c r="E27" s="7"/>
+      <c r="F27" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G27" s="33"/>
+      <c r="G27" s="17"/>
       <c r="J27" s="5" t="b">
         <v>0</v>
       </c>
@@ -2951,21 +2982,21 @@
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="29">
+      <c r="B28" s="6">
         <v>15</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="31">
+      <c r="D28" s="19">
         <v>1</v>
       </c>
-      <c r="E28" s="32"/>
-      <c r="F28" s="29" t="str">
+      <c r="E28" s="7"/>
+      <c r="F28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G28" s="33"/>
+      <c r="G28" s="17"/>
       <c r="J28" s="5" t="b">
         <v>0</v>
       </c>
@@ -2975,21 +3006,21 @@
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="29">
+      <c r="B29" s="6">
         <v>16</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="31">
+      <c r="D29" s="19">
         <v>1</v>
       </c>
-      <c r="E29" s="32"/>
-      <c r="F29" s="29" t="str">
+      <c r="E29" s="7"/>
+      <c r="F29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G29" s="33"/>
+      <c r="G29" s="17"/>
       <c r="J29" s="5" t="b">
         <v>0</v>
       </c>
@@ -2999,21 +3030,21 @@
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="29">
+      <c r="B30" s="6">
         <v>17</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="31">
+      <c r="D30" s="19">
         <v>1</v>
       </c>
-      <c r="E30" s="32"/>
-      <c r="F30" s="29" t="str">
+      <c r="E30" s="7"/>
+      <c r="F30" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G30" s="33"/>
+      <c r="G30" s="17"/>
       <c r="J30" s="5" t="b">
         <v>0</v>
       </c>
@@ -3023,21 +3054,21 @@
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="29">
+      <c r="B31" s="6">
         <v>18</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="31">
+      <c r="D31" s="19">
         <v>1</v>
       </c>
-      <c r="E31" s="32"/>
-      <c r="F31" s="29" t="str">
+      <c r="E31" s="7"/>
+      <c r="F31" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G31" s="33"/>
+      <c r="G31" s="17"/>
       <c r="J31" s="5" t="b">
         <v>0</v>
       </c>
@@ -3047,21 +3078,23 @@
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="29">
+      <c r="B32" s="6">
         <v>19</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="31">
+      <c r="D32" s="19">
         <v>1</v>
       </c>
-      <c r="E32" s="32"/>
-      <c r="F32" s="29" t="str">
+      <c r="E32" s="7"/>
+      <c r="F32" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G32" s="33"/>
+      <c r="G32" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="J32" s="5" t="b">
         <v>0</v>
       </c>
@@ -3071,21 +3104,23 @@
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B33" s="29">
+      <c r="B33" s="6">
         <v>20</v>
       </c>
-      <c r="C33" s="30" t="s">
+      <c r="C33" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="31">
+      <c r="D33" s="19">
         <v>1</v>
       </c>
-      <c r="E33" s="32"/>
-      <c r="F33" s="29" t="str">
+      <c r="E33" s="7"/>
+      <c r="F33" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G33" s="33"/>
+      <c r="G33" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="J33" s="5" t="b">
         <v>0</v>
       </c>
@@ -3095,21 +3130,21 @@
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B34" s="29">
+      <c r="B34" s="6">
         <v>21</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="31">
+      <c r="D34" s="19">
         <v>2</v>
       </c>
-      <c r="E34" s="32"/>
-      <c r="F34" s="29" t="str">
+      <c r="E34" s="7"/>
+      <c r="F34" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G34" s="33"/>
+      <c r="G34" s="17"/>
       <c r="J34" s="5" t="b">
         <v>0</v>
       </c>
@@ -3154,7 +3189,7 @@
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="6" t="str">
-        <f t="shared" ref="F36:F38" si="2">IF(J36,"Done","To Be Done")</f>
+        <f t="shared" ref="F36:F39" si="2">IF(J36,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
       <c r="G36" s="17"/>
@@ -3202,21 +3237,42 @@
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="6" t="str">
+        <f t="shared" ref="F38" si="3">IF(J38,"Done","To Be Done")</f>
+        <v>To Be Done</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B39" s="6">
+        <v>26</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" s="19">
+        <v>0</v>
+      </c>
+      <c r="F39" s="6" t="str">
         <f t="shared" si="2"/>
         <v>To Be Done</v>
       </c>
-      <c r="G38" s="17"/>
-      <c r="J38" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K38" s="2">
+      <c r="G39" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J39" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K39" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="K39" s="2">
-        <f>SUM(K18:K38)</f>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="K40" s="2">
+        <f>SUM(K18:K39)</f>
         <v>0</v>
       </c>
     </row>
@@ -3235,7 +3291,7 @@
       <formula>$F12="Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18:F38">
+  <conditionalFormatting sqref="F18:F39">
     <cfRule type="expression" dxfId="0" priority="6">
       <formula>$F18="Done"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Rotating and Moving Walls
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -1,35 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charm\Workspace\Game Dev I (AGA206)\Roll-A-Ball-Sep-24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdunn9\Workspace\AGA206-Game-Dev-I\Roll-A-Ball-Sep-24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C409F7FF-1237-49B6-851F-C4B14BE6713D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DE3E92-2E31-499C-A3C8-EA6DDF76B072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="2520" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -481,7 +470,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$24" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$24" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
@@ -513,7 +502,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$32" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$32" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2517,8 +2506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2593,7 +2582,7 @@
       </c>
       <c r="D8" s="8">
         <f>COUNTIFS(J18:J39,TRUE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -2602,7 +2591,7 @@
       </c>
       <c r="D9" s="8">
         <f>K40</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2894,17 +2883,17 @@
       <c r="E24" s="7"/>
       <c r="F24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>39</v>
       </c>
       <c r="J24" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
@@ -3090,17 +3079,17 @@
       <c r="E32" s="7"/>
       <c r="F32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G32" s="17" t="s">
         <v>39</v>
       </c>
       <c r="J32" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
@@ -3273,7 +3262,7 @@
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K40" s="2">
         <f>SUM(K18:K39)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3860,16 +3849,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="352e64b8-96de-457a-94b9-e7b41cb76109">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC2262909F271D4783C3CAAEADC83320" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a116d0dcbd67c01ccad3ed0a951122ab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="352e64b8-96de-457a-94b9-e7b41cb76109" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1faf68e6dcd8e517933108d283c31081" ns2:_="">
     <xsd:import namespace="352e64b8-96de-457a-94b9-e7b41cb76109"/>
@@ -4047,6 +4026,16 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="352e64b8-96de-457a-94b9-e7b41cb76109">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4057,16 +4046,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56A7533C-67A9-40BF-8C82-BA3310B920DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="352e64b8-96de-457a-94b9-e7b41cb76109"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7811DB65-6760-4129-AD12-94B5654C992B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4084,6 +4063,16 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56A7533C-67A9-40BF-8C82-BA3310B920DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="352e64b8-96de-457a-94b9-e7b41cb76109"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4E84B29-9993-426F-9193-FF0D475CB0F4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Level Select Menu + World Tilt Mode
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdunn9\Workspace\AGA206-Game-Dev-I\Roll-A-Ball-Sep-24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DE3E92-2E31-499C-A3C8-EA6DDF76B072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A6E738-C7AA-46AA-A5F6-801BC2414B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -542,7 +542,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$18" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$18" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2506,8 +2506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2582,7 +2582,7 @@
       </c>
       <c r="D8" s="8">
         <f>COUNTIFS(J18:J39,TRUE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -2591,7 +2591,7 @@
       </c>
       <c r="D9" s="8">
         <f>K40</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2729,17 +2729,17 @@
       <c r="E18" s="7"/>
       <c r="F18" s="6" t="str">
         <f t="shared" ref="F18:F35" si="0">IF(J18,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>39</v>
       </c>
       <c r="J18" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="2">
         <f>IF(J18=TRUE,D18,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
@@ -3262,7 +3262,7 @@
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K40" s="2">
         <f>SUM(K18:K39)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3849,6 +3849,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="352e64b8-96de-457a-94b9-e7b41cb76109">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC2262909F271D4783C3CAAEADC83320" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a116d0dcbd67c01ccad3ed0a951122ab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="352e64b8-96de-457a-94b9-e7b41cb76109" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1faf68e6dcd8e517933108d283c31081" ns2:_="">
     <xsd:import namespace="352e64b8-96de-457a-94b9-e7b41cb76109"/>
@@ -4026,16 +4036,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="352e64b8-96de-457a-94b9-e7b41cb76109">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4046,6 +4046,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56A7533C-67A9-40BF-8C82-BA3310B920DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="352e64b8-96de-457a-94b9-e7b41cb76109"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7811DB65-6760-4129-AD12-94B5654C992B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4063,16 +4073,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56A7533C-67A9-40BF-8C82-BA3310B920DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="352e64b8-96de-457a-94b9-e7b41cb76109"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4E84B29-9993-426F-9193-FF0D475CB0F4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Tilt level finalized, and development on the health system
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdunn9\Workspace\AGA206-Game-Dev-I\Roll-A-Ball-Sep-24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A6E738-C7AA-46AA-A5F6-801BC2414B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303DE8E4-E8AD-46F2-A36D-3CFE1F6B7170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>AGA206 Assessment 2 Checklist</t>
   </si>
@@ -164,6 +164,24 @@
       </rPr>
       <t>Tonight</t>
     </r>
+  </si>
+  <si>
+    <t>The movement of the ball is abit jankey, need Brendans' Advice. Also need to try and add a rotation limit.</t>
+  </si>
+  <si>
+    <t>Need to make a custom model for the doors</t>
+  </si>
+  <si>
+    <t>Just need to improve the UI Art</t>
+  </si>
+  <si>
+    <t>(Done Early)</t>
+  </si>
+  <si>
+    <t>Health System</t>
+  </si>
+  <si>
+    <t>This Week. I want to add a wash of colour when hit, for a short delay. But cant figure it out.</t>
   </si>
 </sst>
 </file>
@@ -554,7 +572,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1044,8 +1062,8 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
-          <xdr:row>21</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1111,7 +1129,7 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
-          <xdr:row>22</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2049,8 +2067,8 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
-          <xdr:row>36</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:row>35</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2116,7 +2134,7 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
-          <xdr:row>37</xdr:row>
+          <xdr:row>36</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2506,8 +2524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="O27" sqref="O26:O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2582,7 +2600,7 @@
       </c>
       <c r="D8" s="8">
         <f>COUNTIFS(J18:J39,TRUE)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -2591,7 +2609,7 @@
       </c>
       <c r="D9" s="8">
         <f>K40</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2732,7 +2750,7 @@
         <v>Done</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="J18" s="5" t="b">
         <v>1</v>
@@ -2792,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B21" s="6">
         <v>8</v>
       </c>
@@ -2805,17 +2823,17 @@
       <c r="E21" s="7"/>
       <c r="F21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J21" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
@@ -2886,7 +2904,7 @@
         <v>Done</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="J24" s="5" t="b">
         <v>1</v>
@@ -3033,7 +3051,9 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G30" s="17"/>
+      <c r="G30" s="17" t="s">
+        <v>45</v>
+      </c>
       <c r="J30" s="5" t="b">
         <v>0</v>
       </c>
@@ -3082,7 +3102,7 @@
         <v>Done</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="J32" s="5" t="b">
         <v>1</v>
@@ -3166,12 +3186,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B36" s="6">
         <v>23</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D36" s="19">
         <v>2</v>
@@ -3181,7 +3201,9 @@
         <f t="shared" ref="F36:F39" si="2">IF(J36,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="G36" s="17"/>
+      <c r="G36" s="17" t="s">
+        <v>47</v>
+      </c>
       <c r="J36" s="5" t="b">
         <v>0</v>
       </c>
@@ -3262,7 +3284,7 @@
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K40" s="2">
         <f>SUM(K18:K39)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -3460,8 +3482,8 @@
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
-                    <xdr:row>21</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3482,7 +3504,7 @@
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
-                    <xdr:row>22</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -3790,8 +3812,8 @@
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
-                    <xdr:row>36</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
+                    <xdr:row>35</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3812,7 +3834,7 @@
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
-                    <xdr:row>37</xdr:row>
+                    <xdr:row>36</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
@@ -3849,16 +3871,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="352e64b8-96de-457a-94b9-e7b41cb76109">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC2262909F271D4783C3CAAEADC83320" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a116d0dcbd67c01ccad3ed0a951122ab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="352e64b8-96de-457a-94b9-e7b41cb76109" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1faf68e6dcd8e517933108d283c31081" ns2:_="">
     <xsd:import namespace="352e64b8-96de-457a-94b9-e7b41cb76109"/>
@@ -4036,6 +4048,16 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="352e64b8-96de-457a-94b9-e7b41cb76109">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4046,16 +4068,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56A7533C-67A9-40BF-8C82-BA3310B920DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="352e64b8-96de-457a-94b9-e7b41cb76109"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7811DB65-6760-4129-AD12-94B5654C992B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4073,6 +4085,16 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56A7533C-67A9-40BF-8C82-BA3310B920DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="352e64b8-96de-457a-94b9-e7b41cb76109"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4E84B29-9993-426F-9193-FF0D475CB0F4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Rails Fixed, Player Controller Fixed, Post Processing Added, First Build
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdunn9\Workspace\Tri3\Game-Dev-I\Roll-A-Ball-Sep-24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdunn9\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32439257-3B69-493F-9DB6-59569F7521DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381D065F-C565-4313-A0C9-EF3621BFE1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>AGA206 Assessment 2 Checklist</t>
   </si>
@@ -141,54 +141,20 @@
     <t>other models</t>
   </si>
   <si>
-    <t>Joshua Dunn</t>
-  </si>
-  <si>
-    <t>This Week</t>
-  </si>
-  <si>
-    <t>Sketches / Plans for Levels</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This Week </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Tonight</t>
-    </r>
-  </si>
-  <si>
-    <t>The movement of the ball is abit jankey, need Brendans' Advice. Also need to try and add a rotation limit.</t>
-  </si>
-  <si>
-    <t>Need to make a custom model for the doors</t>
-  </si>
-  <si>
-    <t>Just need to improve the UI Art</t>
-  </si>
-  <si>
-    <t>(Done Early)</t>
-  </si>
-  <si>
     <t>Health System</t>
   </si>
   <si>
-    <t>This Week. I want to add a wash of colour when hit, for a short delay. But cant figure it out.</t>
+    <t>Completed in pervious weeks before class</t>
+  </si>
+  <si>
+    <t>Joshua Dunn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -234,8 +200,16 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +225,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -348,7 +328,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -412,6 +392,26 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -492,7 +492,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$25" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$25" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -528,7 +528,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$33" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$33" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
@@ -548,7 +548,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$39" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$38" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -929,7 +929,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -996,7 +996,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1062,8 +1062,8 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1129,8 +1129,8 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
-          <xdr:row>21</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1197,7 +1197,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1264,7 +1264,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1934,7 +1934,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2001,7 +2001,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2067,8 +2067,8 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
-          <xdr:row>35</xdr:row>
-          <xdr:rowOff>200025</xdr:rowOff>
+          <xdr:row>36</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2134,7 +2134,7 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
-          <xdr:row>36</xdr:row>
+          <xdr:row>37</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2522,10 +2522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:L40"/>
+  <dimension ref="B2:L39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2560,12 +2560,12 @@
       <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27"/>
+      <c r="D4" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="34"/>
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
     </row>
@@ -2573,10 +2573,10 @@
       <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="22"/>
       <c r="I5" s="22"/>
     </row>
@@ -2592,15 +2592,14 @@
         <f>COUNTIFS(J12:J15,TRUE)</f>
         <v>4</v>
       </c>
-      <c r="G7"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="8">
-        <f>COUNTIFS(J18:J39,TRUE)</f>
-        <v>5</v>
+        <f>COUNTIFS(J18:J38,TRUE)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -2608,8 +2607,8 @@
         <v>6</v>
       </c>
       <c r="D9" s="8">
-        <f>K40</f>
-        <v>8</v>
+        <f>K39</f>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2688,7 +2687,9 @@
         <f>IF(J14,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="G14" s="17"/>
+      <c r="G14" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="J14" s="5" t="b">
         <v>1</v>
       </c>
@@ -2735,23 +2736,21 @@
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="6">
+      <c r="B18" s="25">
         <v>5</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="27">
         <v>2</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="6" t="str">
+      <c r="E18" s="28"/>
+      <c r="F18" s="25" t="str">
         <f t="shared" ref="F18:F35" si="0">IF(J18,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="G18" s="17" t="s">
-        <v>44</v>
-      </c>
+      <c r="G18" s="29"/>
       <c r="J18" s="5" t="b">
         <v>1</v>
       </c>
@@ -2761,47 +2760,45 @@
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="6">
+      <c r="B19" s="25">
         <v>6</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="27">
         <v>2</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="6" t="str">
-        <f t="shared" si="0"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="31" t="str">
+        <f>IF(J19,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="G19" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="G19" s="29"/>
       <c r="J19" s="5" t="b">
         <v>0</v>
       </c>
       <c r="K19" s="2">
-        <f t="shared" ref="K19:K39" si="1">IF(J19=TRUE,D19,0)</f>
+        <f t="shared" ref="K19:K38" si="1">IF(J19=TRUE,D19,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="6">
+      <c r="B20" s="25">
         <v>7</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="27">
         <v>2</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="6" t="str">
+      <c r="E20" s="28"/>
+      <c r="F20" s="25" t="str">
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="G20" s="17"/>
+      <c r="G20" s="29"/>
       <c r="J20" s="5" t="b">
         <v>1</v>
       </c>
@@ -2810,24 +2807,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B21" s="6">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B21" s="25">
         <v>8</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="27">
         <v>2</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="6" t="str">
+      <c r="E21" s="28"/>
+      <c r="F21" s="25" t="str">
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="G21" s="17" t="s">
-        <v>42</v>
-      </c>
+      <c r="G21" s="29"/>
       <c r="J21" s="5" t="b">
         <v>1</v>
       </c>
@@ -2837,23 +2832,21 @@
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="6">
+      <c r="B22" s="25">
         <v>9</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="27">
         <v>1</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="6" t="str">
+      <c r="E22" s="28"/>
+      <c r="F22" s="25" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G22" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="G22" s="29"/>
       <c r="J22" s="5" t="b">
         <v>0</v>
       </c>
@@ -2863,23 +2856,21 @@
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="6">
+      <c r="B23" s="25">
         <v>10</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="27">
         <v>1</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="6" t="str">
-        <f t="shared" si="0"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="25" t="str">
+        <f>IF(J23,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="G23" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="G23" s="29"/>
       <c r="J23" s="5" t="b">
         <v>0</v>
       </c>
@@ -2889,23 +2880,21 @@
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="6">
+      <c r="B24" s="25">
         <v>11</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="27">
         <v>1</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="6" t="str">
+      <c r="E24" s="28"/>
+      <c r="F24" s="25" t="str">
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="G24" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="G24" s="29"/>
       <c r="J24" s="5" t="b">
         <v>1</v>
       </c>
@@ -2915,47 +2904,45 @@
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="6">
+      <c r="B25" s="25">
         <v>12</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="27">
         <v>1</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="6" t="str">
+      <c r="E25" s="28"/>
+      <c r="F25" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="G25" s="29"/>
+      <c r="J25" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="25">
+        <v>13</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="27">
+        <v>1</v>
+      </c>
+      <c r="E26" s="28"/>
+      <c r="F26" s="25" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G25" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="J25" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K25" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="6">
-        <v>13</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="19">
-        <v>1</v>
-      </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G26" s="17"/>
+      <c r="G26" s="29"/>
       <c r="J26" s="5" t="b">
         <v>0</v>
       </c>
@@ -2965,21 +2952,21 @@
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="6">
+      <c r="B27" s="25">
         <v>14</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="19">
+      <c r="D27" s="27">
         <v>1</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="6" t="str">
+      <c r="E27" s="28"/>
+      <c r="F27" s="25" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G27" s="17"/>
+      <c r="G27" s="29"/>
       <c r="J27" s="5" t="b">
         <v>0</v>
       </c>
@@ -2989,21 +2976,21 @@
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="6">
+      <c r="B28" s="25">
         <v>15</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="19">
+      <c r="D28" s="27">
         <v>1</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="6" t="str">
+      <c r="E28" s="28"/>
+      <c r="F28" s="25" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G28" s="17"/>
+      <c r="G28" s="29"/>
       <c r="J28" s="5" t="b">
         <v>0</v>
       </c>
@@ -3013,21 +3000,21 @@
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="6">
+      <c r="B29" s="25">
         <v>16</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="19">
+      <c r="D29" s="27">
         <v>1</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="6" t="str">
+      <c r="E29" s="28"/>
+      <c r="F29" s="25" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G29" s="17"/>
+      <c r="G29" s="29"/>
       <c r="J29" s="5" t="b">
         <v>0</v>
       </c>
@@ -3037,23 +3024,21 @@
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="6">
+      <c r="B30" s="25">
         <v>17</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="19">
+      <c r="D30" s="27">
         <v>1</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="6" t="str">
+      <c r="E30" s="28"/>
+      <c r="F30" s="25" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G30" s="17" t="s">
-        <v>45</v>
-      </c>
+      <c r="G30" s="29"/>
       <c r="J30" s="5" t="b">
         <v>0</v>
       </c>
@@ -3063,21 +3048,21 @@
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="6">
+      <c r="B31" s="25">
         <v>18</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="19">
+      <c r="D31" s="27">
         <v>1</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="6" t="str">
+      <c r="E31" s="28"/>
+      <c r="F31" s="25" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G31" s="17"/>
+      <c r="G31" s="29"/>
       <c r="J31" s="5" t="b">
         <v>0</v>
       </c>
@@ -3087,23 +3072,21 @@
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="6">
+      <c r="B32" s="25">
         <v>19</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="19">
+      <c r="D32" s="27">
         <v>1</v>
       </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="6" t="str">
+      <c r="E32" s="28"/>
+      <c r="F32" s="25" t="str">
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="G32" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="G32" s="29"/>
       <c r="J32" s="5" t="b">
         <v>1</v>
       </c>
@@ -3113,47 +3096,45 @@
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B33" s="6">
+      <c r="B33" s="25">
         <v>20</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="19">
+      <c r="D33" s="27">
         <v>1</v>
       </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="6" t="str">
+      <c r="E33" s="28"/>
+      <c r="F33" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="G33" s="29"/>
+      <c r="J33" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K33" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B34" s="25">
+        <v>21</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="27">
+        <v>2</v>
+      </c>
+      <c r="E34" s="28"/>
+      <c r="F34" s="25" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G33" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="J33" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K33" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B34" s="6">
-        <v>21</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="19">
-        <v>2</v>
-      </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G34" s="17"/>
+      <c r="G34" s="29"/>
       <c r="J34" s="5" t="b">
         <v>0</v>
       </c>
@@ -3186,24 +3167,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="6">
         <v>23</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D36" s="19">
         <v>2</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="6" t="str">
-        <f t="shared" ref="F36:F39" si="2">IF(J36,"Done","To Be Done")</f>
+        <f t="shared" ref="F36:F38" si="2">IF(J36,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="G36" s="17" t="s">
-        <v>47</v>
-      </c>
+      <c r="G36" s="17"/>
       <c r="J36" s="5" t="b">
         <v>0</v>
       </c>
@@ -3248,43 +3227,22 @@
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="6" t="str">
-        <f t="shared" ref="F38" si="3">IF(J38,"Done","To Be Done")</f>
-        <v>To Be Done</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="J38" s="5"/>
+        <f t="shared" si="2"/>
+        <v>Done</v>
+      </c>
+      <c r="G38" s="17"/>
+      <c r="J38" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K38" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B39" s="6">
-        <v>26</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D39" s="19">
-        <v>0</v>
-      </c>
-      <c r="F39" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J39" s="5" t="b">
-        <v>0</v>
-      </c>
       <c r="K39" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="K40" s="2">
-        <f>SUM(K18:K39)</f>
-        <v>8</v>
+        <f>SUM(K18:K38)</f>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -3302,7 +3260,7 @@
       <formula>$F12="Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18:F39">
+  <conditionalFormatting sqref="F18:F38">
     <cfRule type="expression" dxfId="0" priority="6">
       <formula>$F18="Done"</formula>
     </cfRule>
@@ -3439,7 +3397,7 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>19</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3461,7 +3419,7 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>20</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3482,8 +3440,8 @@
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
-                    <xdr:row>20</xdr:row>
-                    <xdr:rowOff>190500</xdr:rowOff>
+                    <xdr:row>21</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3504,8 +3462,8 @@
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
-                    <xdr:row>21</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:row>22</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3527,7 +3485,7 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>23</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3549,7 +3507,7 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>24</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3769,7 +3727,7 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>34</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3791,7 +3749,7 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>35</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3812,8 +3770,8 @@
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
-                    <xdr:row>35</xdr:row>
-                    <xdr:rowOff>200025</xdr:rowOff>
+                    <xdr:row>36</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3834,7 +3792,7 @@
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
-                    <xdr:row>36</xdr:row>
+                    <xdr:row>37</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
@@ -3871,16 +3829,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="352e64b8-96de-457a-94b9-e7b41cb76109">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC2262909F271D4783C3CAAEADC83320" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a116d0dcbd67c01ccad3ed0a951122ab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="352e64b8-96de-457a-94b9-e7b41cb76109" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1faf68e6dcd8e517933108d283c31081" ns2:_="">
     <xsd:import namespace="352e64b8-96de-457a-94b9-e7b41cb76109"/>
@@ -4058,6 +4006,16 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="352e64b8-96de-457a-94b9-e7b41cb76109">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4068,16 +4026,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56A7533C-67A9-40BF-8C82-BA3310B920DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="352e64b8-96de-457a-94b9-e7b41cb76109"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7811DB65-6760-4129-AD12-94B5654C992B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4095,6 +4043,16 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56A7533C-67A9-40BF-8C82-BA3310B920DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="352e64b8-96de-457a-94b9-e7b41cb76109"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4E84B29-9993-426F-9193-FF0D475CB0F4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Powerups Fixed, UI started
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -1,35 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charm\Workspace\Game Dev I (AGA206)\Roll-A-Ball-Sep-24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdunn9\Workspace\AGA206-Game-Dev-I\Roll-A-Ball-Sep-24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1613E104-859B-44C1-9B04-8AD1EC71F337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A4813A-1CF6-4761-AB7C-E3AF2DB53973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="2520" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -146,9 +135,6 @@
     <t>particle effects to pick ups</t>
   </si>
   <si>
-    <t>Come up with your own</t>
-  </si>
-  <si>
     <t>other models</t>
   </si>
   <si>
@@ -159,6 +145,9 @@
   </si>
   <si>
     <t>Joshua Dunn</t>
+  </si>
+  <si>
+    <t>LERPING Or Animating Bumpers</t>
   </si>
 </sst>
 </file>
@@ -507,15 +496,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$26" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$26" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$27" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$27" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$28" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$28" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2535,8 +2524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A20" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2572,7 +2561,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="33"/>
       <c r="F4" s="33"/>
@@ -2610,7 +2599,7 @@
       </c>
       <c r="D8" s="8">
         <f>COUNTIFS(J18:J38,TRUE)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -2619,7 +2608,7 @@
       </c>
       <c r="D9" s="8">
         <f>K39</f>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2699,7 +2688,7 @@
         <v>Done</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J14" s="5" t="b">
         <v>1</v>
@@ -2951,15 +2940,15 @@
       <c r="E26" s="28"/>
       <c r="F26" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G26" s="29"/>
       <c r="J26" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
@@ -2975,15 +2964,15 @@
       <c r="E27" s="28"/>
       <c r="F27" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G27" s="29"/>
       <c r="J27" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
@@ -2999,15 +2988,15 @@
       <c r="E28" s="28"/>
       <c r="F28" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G28" s="29"/>
       <c r="J28" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
@@ -3183,7 +3172,7 @@
         <v>23</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D36" s="19">
         <v>2</v>
@@ -3207,7 +3196,7 @@
         <v>24</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D37" s="19">
         <v>1</v>
@@ -3231,7 +3220,7 @@
         <v>25</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38" s="19">
         <v>1</v>
@@ -3253,7 +3242,7 @@
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K39" s="2">
         <f>SUM(K18:K38)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -3840,6 +3829,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC2262909F271D4783C3CAAEADC83320" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a116d0dcbd67c01ccad3ed0a951122ab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="352e64b8-96de-457a-94b9-e7b41cb76109" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1faf68e6dcd8e517933108d283c31081" ns2:_="">
     <xsd:import namespace="352e64b8-96de-457a-94b9-e7b41cb76109"/>
@@ -4017,15 +4015,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4037,6 +4026,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4E84B29-9993-426F-9193-FF0D475CB0F4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7811DB65-6760-4129-AD12-94B5654C992B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4054,14 +4051,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4E84B29-9993-426F-9193-FF0D475CB0F4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56A7533C-67A9-40BF-8C82-BA3310B920DD}">
   <ds:schemaRefs>

</xml_diff>